<commit_message>
Added new biomodels as sympy equations to the correct_eqs.tsv database
</commit_message>
<xml_diff>
--- a/notebooks/equation extraction development/extraction error check/string mismatch check/correct_eqs_list_EXCEL.xlsx
+++ b/notebooks/equation extraction development/extraction error check/string mismatch check/correct_eqs_list_EXCEL.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kovacs.f/Desktop/mira/notebooks/equation extraction development/extraction error check/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kovacs.f/Desktop/mira/notebooks/equation extraction development/extraction error check/string mismatch check/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D513B96-6ADA-6040-BEBE-B12E60F5C385}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC360E7-291B-DC46-BA2E-918A063F91FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-51200" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{30A3DCF3-ADF7-634A-A177-E80CD8B6545B}"/>
+    <workbookView xWindow="-51200" yWindow="0" windowWidth="22880" windowHeight="28800" xr2:uid="{30A3DCF3-ADF7-634A-A177-E80CD8B6545B}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>model</t>
   </si>
@@ -181,6 +181,165 @@
     sympy.Eq(T(t).diff(t), mu * A(t) + nu * R(t) - (sigma + tau) * T(t)),
     sympy.Eq(H(t).diff(t), lambda_ * I(t) + rho * D(t) + kappa * A(t) + xi * R(t) + sigma * T(t)),
     sympy.Eq(E(t).diff(t), tau * T(t))
+]</t>
+  </si>
+  <si>
+    <t>BIOMD0000000963</t>
+  </si>
+  <si>
+    <t>odes = [
+    sympy.Eq(S(t).diff(t), - beta * (S*I / (1+alpha*R)),
+    sympy.Eq(I(t).diff(t), beta * (S*I / (1+alpha*R) - gamma*I),
+    sympy.Eq(R(t).diff(t), gamma*I),
+  ]</t>
+  </si>
+  <si>
+    <t>BIOMD0000000964</t>
+  </si>
+  <si>
+    <t>odes = [
+    sympy.Eq(S(t).diff(t), b - (beta_1*S*P)/(1+alpha_1*P) - (beta_2*S*(I_A,+,I_S))/(1+alpha_2*(I_A,+,I_S)) + psi*E - mu*S),
+    sympy.Eq(E(t).diff(t), (beta_1*S*P)/(1+alpha_1*P) + (beta_2*S*(I_A,+,I_S))/(1+alpha_2*(I_A,+,I_S)) - psi*E - mu*E - omega*E),
+    sympy.Eq(I_A(t).diff(t), (1-delta)*omega*E - (mu+sigma)*I_A - gamma_A*I_A),
+    sympy.Eq(I_S(t).diff(t), delta*omega*E - (mu+sigma)*I_S - gamma_S*I_S),
+    sympy.Eq(R(t).diff(t), gamma_S*I_S + gamma_A*I_A - mu*R),
+    sympy.Eq(P(t).diff(t), eta_A*I_A + eta_S*I_S - mu_p*P)
+  ]</t>
+  </si>
+  <si>
+    <t>BIOMD0000000970</t>
+  </si>
+  <si>
+    <t>odes = [
+    sympy.Eq(S(t).diff(t), -r_1*beta_1*I*S/N - r_2*beta_2*E*S/N),
+    sympy.Eq(E(t).diff(t), r_1*beta*I*S/N - alpha*E + r_2*beta_2*E*S/N),
+    sympy.Eq(I(t).diff(t), alpha*E - gamma*I),
+    sympy.Eq(R(t).diff(t), gamma*I)
+]</t>
+  </si>
+  <si>
+    <t>BIOMD0000000971</t>
+  </si>
+  <si>
+    <t>odes = [
+    sympy.Eq(S(t).diff(t), -(beta*c + c*q*(1 - beta))*S*(I + theta*A) + lambda_*S_q),
+    sympy.Eq(E(t).diff(t), beta*c*(1 - q)*S*(I + theta*A) - sigma*E),
+    sympy.Eq(I(t).diff(t), sigma*rho*E - (delta_I + alpha + gamma_I)*I),
+    sympy.Eq(A(t).diff(t), sigma*(1 - rho)*E - gamma_A*A),
+    sympy.Eq(S_q(t).diff(t), (1 - beta)*c*q*S*(I + theta*A) - lambda_*S_q),
+    sympy.Eq(E_q(t).diff(t), beta*c*q*S*(I + theta*A) - delta_q*E_q),
+    sympy.Eq(H(t).diff(t), delta_I*I + delta_q*E_q - (alpha + gamma_H)*H),
+    sympy.Eq(R(t).diff(t), gamma_I*I + gamma_A*A + gamma_H*H)
+]</t>
+  </si>
+  <si>
+    <t>BIOMD0000000972</t>
+  </si>
+  <si>
+    <t>odes = [
+    sympy.Eq(S(t).diff(t), -(beta*c(t) + c(t)*q*(1 - beta))*S*(I + theta*A) + lambda_*S_q),
+    sympy.Eq(E(t).diff(t), beta*c(t)*(1 - q)*S*(I + theta*A) - sigma*E),
+    sympy.Eq(I(t).diff(t), sigma*rho*E - (delta_I(t) + alpha + gamma_I)*I),
+    sympy.Eq(A(t).diff(t), sigma*(1 - rho)*E - gamma_A*A),
+    sympy.Eq(S_q(t).diff(t), (1 - beta)*c(t)*q*S*(I + theta*A) - lambda_*S_q),
+    sympy.Eq(E_q(t).diff(t), beta*c(t)*q*S*(I + theta*A) - delta_q*E_q),
+    sympy.Eq(H(t).diff(t), delta_I(t)*I + delta_q*E_q - (alpha + gamma_H)*H),
+    sympy.Eq(R(t).diff(t), gamma_I*I + gamma_A*A + gamma_H*H)
+]</t>
+  </si>
+  <si>
+    <t>BIOMD0000000974</t>
+  </si>
+  <si>
+    <t>BIOMD0000000976</t>
+  </si>
+  <si>
+    <t>BIOMD0000000977</t>
+  </si>
+  <si>
+    <t>odes = [
+    sympy.Eq(S(t).diff(t), Lambda - mu*S - beta*S*I/N),
+    sympy.Eq(E(t).diff(t), beta*S*I/N - (mu + epsilon)*E),
+    sympy.Eq(I(t).diff(t), epsilon*E - (gamma + mu + alpha)*I),
+    sympy.Eq(R(t).diff(t), gamma*I - mu*R)
+]</t>
+  </si>
+  <si>
+    <t>odes = [
+    sympy.Eq(S(t).diff(t), -tau(t)*S(t)*(I_1(t) + I_2(t))),
+    sympy.Eq(I_1(t).diff(t), alpha*tau(t)*S(t)*(I_1(t) + I_2(t)) - gamma_1*I_1(t)),
+    sympy.Eq(I_2(t).diff(t), (1 - alpha)*tau(t)*S(t)*(I_1(t) + I_2(t)) - (gamma_2 + mu)*I_2(t)),
+    sympy.Eq(R(t).diff(t), gamma_1*I_1(t) + gamma_2*I_2(t))
+]</t>
+  </si>
+  <si>
+    <t>odes = [
+    sympy.Eq(S(t).diff(t), Lambda_s - (beta_s + rho_s*(1 - beta_s))*epsilon_s*S*I/N - delta*S + m_s*S_q),
+    sympy.Eq(S_q(t).diff(t), (1 - beta_s)*epsilon_s*rho_s*S*I/N - (m_s + delta)*S_q),
+    sympy.Eq(A(t).diff(t), beta_s*(1 - rho_s)*epsilon_s*S*I/N - (gamma_a + xi_a + delta)*A),
+    sympy.Eq(I(t).diff(t), gamma_a*A - (gamma_i + xi_i + delta)*I),
+    sympy.Eq(I_q(t).diff(t), beta_s*epsilon_s*rho_s*S*I/N + gamma_i*I - (xi_q + delta)*I_q),
+    sympy.Eq(R(t).diff(t), xi_a*A + xi_i*I + xi_q*I_q - delta*R)
+]</t>
+  </si>
+  <si>
+    <t>BIOMD0000000978</t>
+  </si>
+  <si>
+    <t>BIOMD0000000979</t>
+  </si>
+  <si>
+    <t>odes = [
+    sympy.Eq(S(t).diff(t), -(1 - epsilon)*beta*S*I/N),
+    sympy.Eq(E(t).diff(t), (1 - epsilon)*beta*S*I/N - sigma*E),
+    sympy.Eq(I(t).diff(t), sigma*E - gamma*I),
+    sympy.Eq(R(t).diff(t), gamma*I)
+]</t>
+  </si>
+  <si>
+    <t>odes = [
+    sympy.Eq(S(t).diff(t), -beta(t)*S(t)/N*I(t) + omega*R(t)),
+    sympy.Eq(E(t).diff(t), beta(t)*S(t)*/N*I(t) - sigma*E(t)),
+    sympy.Eq(I(t).diff(t), sigma*E(t) - gamma*I(t)),
+    sympy.Eq(R(t).diff(t), gamma*I(t) - omega*R(t))
+]</t>
+  </si>
+  <si>
+    <t>BIOMD0000000984</t>
+  </si>
+  <si>
+    <t>odes = [
+    sympy.Eq(S_c(t).diff(t), m(t)*S_u - (1 - m(t))*S_c),
+    sympy.Eq(S_u(t).diff(t), (1 - m(t))*S_c - m(t)*S_u - beta*(n*I_r + I_u)*S_u + theta*(1 - lambda_)*Q),
+    sympy.Eq(E(t).diff(t), (1 - sigma)*beta*(n*I_r + I_u)*S_u - mu*E),
+    sympy.Eq(I_r(t).diff(t), mu*f*E + theta*lambda*Q - eta_r*I_r),
+    sympy.Eq(I_u(t).diff(t), mu*(1 - f)*E - eta_u*I_u),
+    sympy.Eq(R(t).diff(t), eta_r*q*I_r + eta_u*I_u),
+    sympy.Eq(Q(t).diff(t), sigma*beta*(n*I_r + I_u)*S_u - theta*Q)
+]</t>
+  </si>
+  <si>
+    <t>BIOMD0000000983</t>
+  </si>
+  <si>
+    <t>BIOMD0000000991A</t>
+  </si>
+  <si>
+    <t>odes = [
+    sympy.Eq(S(t).diff(t), -beta*S/N*I),
+    sympy.Eq(E(t).diff(t), beta*S/N*I - omega*E),
+    sympy.Eq(I(t).diff(t), omega*E - gamma*I),
+    sympy.Eq(R(t).diff(t), gamma*I)
+]</t>
+  </si>
+  <si>
+    <t>odes = [
+    sympy.Eq(S(t).diff(t), -beta_c*(alpha*A + I)*S/(N_h - I_D)),
+    sympy.Eq(E(t).diff(t), beta_c*(alpha*A + I)*S/(N_h - I_D) - sigma*E),
+    sympy.Eq(A(t).diff(t), nu*sigma*E - (theta + gamma_a)*A),
+    sympy.Eq(I(t).diff(t), (1 - nu)*sigma*E - (psi + gamma_O + d_O)*I),
+    sympy.Eq(I_D(t).diff(t), theta*A + psi*I - (gamma_i + d_D)*I_D),
+    sympy.Eq(R(t).diff(t), gamma_i*I_D + gamma_a*A + gamma_O*I)
 ]</t>
   </si>
 </sst>
@@ -577,16 +736,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{585F8C20-F92E-4147-81E7-1FDA03FC9F94}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="B21" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="107.83203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="68.5" style="2" customWidth="1"/>
     <col min="3" max="3" width="83.1640625" style="2" customWidth="1"/>
     <col min="4" max="16384" width="10.83203125" style="2"/>
   </cols>
@@ -671,12 +830,116 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="153" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="170" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="85" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="170" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="102" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="170" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="187" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="102" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="119" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="187" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="102" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="102" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="170" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="102" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="136" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Small changes and more results
</commit_message>
<xml_diff>
--- a/notebooks/equation extraction development/extraction error check/string mismatch check/correct_eqs_list_EXCEL.xlsx
+++ b/notebooks/equation extraction development/extraction error check/string mismatch check/correct_eqs_list_EXCEL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kovacs.f/Desktop/mira/notebooks/equation extraction development/extraction error check/string mismatch check/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC360E7-291B-DC46-BA2E-918A063F91FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D0CC7C6-92C3-874F-86CC-ACE424EF1E93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-51200" yWindow="0" windowWidth="22880" windowHeight="28800" xr2:uid="{30A3DCF3-ADF7-634A-A177-E80CD8B6545B}"/>
+    <workbookView xWindow="4440" yWindow="760" windowWidth="25800" windowHeight="17180" xr2:uid="{30A3DCF3-ADF7-634A-A177-E80CD8B6545B}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -322,9 +322,6 @@
     <t>BIOMD0000000983</t>
   </si>
   <si>
-    <t>BIOMD0000000991A</t>
-  </si>
-  <si>
     <t>odes = [
     sympy.Eq(S(t).diff(t), -beta*S/N*I),
     sympy.Eq(E(t).diff(t), beta*S/N*I - omega*E),
@@ -341,6 +338,9 @@
     sympy.Eq(I_D(t).diff(t), theta*A + psi*I - (gamma_i + d_D)*I_D),
     sympy.Eq(R(t).diff(t), gamma_i*I_D + gamma_a*A + gamma_O*I)
 ]</t>
+  </si>
+  <si>
+    <t>BIOMD0000000991</t>
   </si>
 </sst>
 </file>
@@ -738,8 +738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{585F8C20-F92E-4147-81E7-1FDA03FC9F94}">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B21" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -931,15 +931,15 @@
         <v>42</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="136" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed loop for function/symbol recognition, edited prompt to avoid overcorrecting, added detailed instructions about common mistakes
</commit_message>
<xml_diff>
--- a/notebooks/equation extraction development/extraction error check/string mismatch check/correct_eqs_list_EXCEL.xlsx
+++ b/notebooks/equation extraction development/extraction error check/string mismatch check/correct_eqs_list_EXCEL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10817"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kovacs.f/Desktop/mira/notebooks/equation extraction development/extraction error check/string mismatch check/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D0CC7C6-92C3-874F-86CC-ACE424EF1E93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB814EC7-C16A-DD46-9248-3705453F5310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="760" windowWidth="25800" windowHeight="17180" xr2:uid="{30A3DCF3-ADF7-634A-A177-E80CD8B6545B}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{30A3DCF3-ADF7-634A-A177-E80CD8B6545B}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -738,8 +738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{585F8C20-F92E-4147-81E7-1FDA03FC9F94}">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -782,7 +782,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="170" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="255" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Updates: results of odes comparison
</commit_message>
<xml_diff>
--- a/notebooks/equation extraction development/extraction error check/string mismatch check/correct_eqs_list_EXCEL.xlsx
+++ b/notebooks/equation extraction development/extraction error check/string mismatch check/correct_eqs_list_EXCEL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kovacs.f/Desktop/mira/notebooks/equation extraction development/extraction error check/string mismatch check/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB814EC7-C16A-DD46-9248-3705453F5310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2880D55-8CB4-4543-A0C8-08B28E6AC7B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{30A3DCF3-ADF7-634A-A177-E80CD8B6545B}"/>
+    <workbookView xWindow="4440" yWindow="760" windowWidth="15000" windowHeight="17180" xr2:uid="{30A3DCF3-ADF7-634A-A177-E80CD8B6545B}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -738,8 +738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{585F8C20-F92E-4147-81E7-1FDA03FC9F94}">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -758,7 +758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="170" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="221" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -806,7 +806,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="238" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="255" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -814,7 +814,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="204" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="238" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
Finalized version with the implementation of iterative architecture for equation extraction
</commit_message>
<xml_diff>
--- a/notebooks/equation extraction development/extraction error check/string mismatch check/correct_eqs_list_EXCEL.xlsx
+++ b/notebooks/equation extraction development/extraction error check/string mismatch check/correct_eqs_list_EXCEL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kovacs.f/Desktop/mira/notebooks/equation extraction development/extraction error check/string mismatch check/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2880D55-8CB4-4543-A0C8-08B28E6AC7B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{693F7189-3C59-6545-AAB2-7918B630095A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="760" windowWidth="15000" windowHeight="17180" xr2:uid="{30A3DCF3-ADF7-634A-A177-E80CD8B6545B}"/>
+    <workbookView xWindow="-35780" yWindow="2440" windowWidth="22220" windowHeight="20500" xr2:uid="{30A3DCF3-ADF7-634A-A177-E80CD8B6545B}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -187,67 +187,18 @@
     <t>BIOMD0000000963</t>
   </si>
   <si>
-    <t>odes = [
-    sympy.Eq(S(t).diff(t), - beta * (S*I / (1+alpha*R)),
-    sympy.Eq(I(t).diff(t), beta * (S*I / (1+alpha*R) - gamma*I),
-    sympy.Eq(R(t).diff(t), gamma*I),
-  ]</t>
-  </si>
-  <si>
     <t>BIOMD0000000964</t>
   </si>
   <si>
-    <t>odes = [
-    sympy.Eq(S(t).diff(t), b - (beta_1*S*P)/(1+alpha_1*P) - (beta_2*S*(I_A,+,I_S))/(1+alpha_2*(I_A,+,I_S)) + psi*E - mu*S),
-    sympy.Eq(E(t).diff(t), (beta_1*S*P)/(1+alpha_1*P) + (beta_2*S*(I_A,+,I_S))/(1+alpha_2*(I_A,+,I_S)) - psi*E - mu*E - omega*E),
-    sympy.Eq(I_A(t).diff(t), (1-delta)*omega*E - (mu+sigma)*I_A - gamma_A*I_A),
-    sympy.Eq(I_S(t).diff(t), delta*omega*E - (mu+sigma)*I_S - gamma_S*I_S),
-    sympy.Eq(R(t).diff(t), gamma_S*I_S + gamma_A*I_A - mu*R),
-    sympy.Eq(P(t).diff(t), eta_A*I_A + eta_S*I_S - mu_p*P)
-  ]</t>
-  </si>
-  <si>
     <t>BIOMD0000000970</t>
   </si>
   <si>
-    <t>odes = [
-    sympy.Eq(S(t).diff(t), -r_1*beta_1*I*S/N - r_2*beta_2*E*S/N),
-    sympy.Eq(E(t).diff(t), r_1*beta*I*S/N - alpha*E + r_2*beta_2*E*S/N),
-    sympy.Eq(I(t).diff(t), alpha*E - gamma*I),
-    sympy.Eq(R(t).diff(t), gamma*I)
-]</t>
-  </si>
-  <si>
     <t>BIOMD0000000971</t>
   </si>
   <si>
-    <t>odes = [
-    sympy.Eq(S(t).diff(t), -(beta*c + c*q*(1 - beta))*S*(I + theta*A) + lambda_*S_q),
-    sympy.Eq(E(t).diff(t), beta*c*(1 - q)*S*(I + theta*A) - sigma*E),
-    sympy.Eq(I(t).diff(t), sigma*rho*E - (delta_I + alpha + gamma_I)*I),
-    sympy.Eq(A(t).diff(t), sigma*(1 - rho)*E - gamma_A*A),
-    sympy.Eq(S_q(t).diff(t), (1 - beta)*c*q*S*(I + theta*A) - lambda_*S_q),
-    sympy.Eq(E_q(t).diff(t), beta*c*q*S*(I + theta*A) - delta_q*E_q),
-    sympy.Eq(H(t).diff(t), delta_I*I + delta_q*E_q - (alpha + gamma_H)*H),
-    sympy.Eq(R(t).diff(t), gamma_I*I + gamma_A*A + gamma_H*H)
-]</t>
-  </si>
-  <si>
     <t>BIOMD0000000972</t>
   </si>
   <si>
-    <t>odes = [
-    sympy.Eq(S(t).diff(t), -(beta*c(t) + c(t)*q*(1 - beta))*S*(I + theta*A) + lambda_*S_q),
-    sympy.Eq(E(t).diff(t), beta*c(t)*(1 - q)*S*(I + theta*A) - sigma*E),
-    sympy.Eq(I(t).diff(t), sigma*rho*E - (delta_I(t) + alpha + gamma_I)*I),
-    sympy.Eq(A(t).diff(t), sigma*(1 - rho)*E - gamma_A*A),
-    sympy.Eq(S_q(t).diff(t), (1 - beta)*c(t)*q*S*(I + theta*A) - lambda_*S_q),
-    sympy.Eq(E_q(t).diff(t), beta*c(t)*q*S*(I + theta*A) - delta_q*E_q),
-    sympy.Eq(H(t).diff(t), delta_I(t)*I + delta_q*E_q - (alpha + gamma_H)*H),
-    sympy.Eq(R(t).diff(t), gamma_I*I + gamma_A*A + gamma_H*H)
-]</t>
-  </si>
-  <si>
     <t>BIOMD0000000974</t>
   </si>
   <si>
@@ -255,14 +206,6 @@
   </si>
   <si>
     <t>BIOMD0000000977</t>
-  </si>
-  <si>
-    <t>odes = [
-    sympy.Eq(S(t).diff(t), Lambda - mu*S - beta*S*I/N),
-    sympy.Eq(E(t).diff(t), beta*S*I/N - (mu + epsilon)*E),
-    sympy.Eq(I(t).diff(t), epsilon*E - (gamma + mu + alpha)*I),
-    sympy.Eq(R(t).diff(t), gamma*I - mu*R)
-]</t>
   </si>
   <si>
     <t>odes = [
@@ -273,74 +216,131 @@
 ]</t>
   </si>
   <si>
-    <t>odes = [
-    sympy.Eq(S(t).diff(t), Lambda_s - (beta_s + rho_s*(1 - beta_s))*epsilon_s*S*I/N - delta*S + m_s*S_q),
-    sympy.Eq(S_q(t).diff(t), (1 - beta_s)*epsilon_s*rho_s*S*I/N - (m_s + delta)*S_q),
-    sympy.Eq(A(t).diff(t), beta_s*(1 - rho_s)*epsilon_s*S*I/N - (gamma_a + xi_a + delta)*A),
-    sympy.Eq(I(t).diff(t), gamma_a*A - (gamma_i + xi_i + delta)*I),
-    sympy.Eq(I_q(t).diff(t), beta_s*epsilon_s*rho_s*S*I/N + gamma_i*I - (xi_q + delta)*I_q),
-    sympy.Eq(R(t).diff(t), xi_a*A + xi_i*I + xi_q*I_q - delta*R)
-]</t>
-  </si>
-  <si>
     <t>BIOMD0000000978</t>
   </si>
   <si>
     <t>BIOMD0000000979</t>
   </si>
   <si>
-    <t>odes = [
-    sympy.Eq(S(t).diff(t), -(1 - epsilon)*beta*S*I/N),
-    sympy.Eq(E(t).diff(t), (1 - epsilon)*beta*S*I/N - sigma*E),
-    sympy.Eq(I(t).diff(t), sigma*E - gamma*I),
-    sympy.Eq(R(t).diff(t), gamma*I)
+    <t>BIOMD0000000984</t>
+  </si>
+  <si>
+    <t>BIOMD0000000983</t>
+  </si>
+  <si>
+    <t>BIOMD0000000991</t>
+  </si>
+  <si>
+    <t>odes = [
+    sympy.Eq(S(t).diff(t), -beta * S(t) * I(t) / (1 + alpha*R(t))),
+    sympy.Eq(I(t).diff(t), beta * S(t) * I(t) / (1 + alpha*R(t)) - gamma*I(t)),
+    sympy.Eq(R(t).diff(t), gamma*I(t))
+]</t>
+  </si>
+  <si>
+    <t>odes = [
+    sympy.Eq(S(t).diff(t), b - (beta_1*S(t)*P(t))/(1+alpha_1*P(t)) - (beta_2*S(t)*(I_A(t)+I_S(t)))/(1+alpha_2*(I_A(t)+I_S(t))) + psi*E(t) - mu*S(t)),
+    sympy.Eq(E(t).diff(t), (beta_1*S(t)*P(t))/(1+alpha_1*P(t)) + (beta_2*S(t)*(I_A(t)+I_S(t)))/(1+alpha_2*(I_A(t)+I_S(t))) - psi*E(t) - mu*E(t) - omega*E(t)),
+    sympy.Eq(I_A(t).diff(t), (1-delta)*omega*E(t) - (mu+sigma)*I_A(t) - gamma_A*I_A(t)),
+    sympy.Eq(I_S(t).diff(t), delta*omega*E(t) - (mu+sigma)*I_S(t) - gamma_S*I_S(t)),
+    sympy.Eq(R(t).diff(t), gamma_S*I_S(t) + gamma_A*I_A(t) - mu*R(t)),
+    sympy.Eq(P(t).diff(t), eta_A*I_A(t) + eta_S*I_S(t) - mu_p*P(t))
+]</t>
+  </si>
+  <si>
+    <t>odes = [
+    sympy.Eq(S(t).diff(t), -r_1*beta_1*I(t)*S(t)/N - r_2*beta_2*E(t)*S(t)/N),
+    sympy.Eq(E(t).diff(t), r_1*beta*I(t)*S(t)/N - alpha*E(t) + r_2*beta_2*E(t)*S(t)/N),
+    sympy.Eq(I(t).diff(t), alpha*E(t) - gamma*I(t)),
+    sympy.Eq(R(t).diff(t), gamma*I(t))
+]</t>
+  </si>
+  <si>
+    <t>odes = [
+    sympy.Eq(S(t).diff(t), -(beta*c + c*q*(1 - beta))*S(t)*(I(t) + theta*A(t)) + lambda_*S_q(t)),
+    sympy.Eq(E(t).diff(t), beta*c*(1 - q)*S(t)*(I(t) + theta*A(t)) - sigma*E(t)),
+    sympy.Eq(I(t).diff(t), sigma*rho*E(t) - (delta_I + alpha + gamma_I)*I(t)),
+    sympy.Eq(A(t).diff(t), sigma*(1 - rho)*E(t) - gamma_A*A(t)),
+    sympy.Eq(S_q(t).diff(t), (1 - beta)*c*q*S(t)*(I(t) + theta*A(t)) - lambda_*S_q(t)),
+    sympy.Eq(E_q(t).diff(t), beta*c*q*S(t)*(I(t) + theta*A(t)) - delta_q*E_q(t)),
+    sympy.Eq(H(t).diff(t), delta_I*I(t) + delta_q*E_q(t) - (alpha + gamma_H)*H(t)),
+    sympy.Eq(R(t).diff(t), gamma_I*I(t) + gamma_A*A(t) + gamma_H*H(t))
+]</t>
+  </si>
+  <si>
+    <t>odes = [
+    sympy.Eq(S(t).diff(t), -(beta*c(t) + c(t)*q*(1 - beta))*S(t)*(I(t) + theta*A(t)) + lambda_*S_q(t)),
+    sympy.Eq(E(t).diff(t), beta*c(t)*(1 - q)*S(t)*(I(t) + theta*A(t)) - sigma*E(t)),
+    sympy.Eq(I(t).diff(t), sigma*rho*E(t) - (delta_I(t) + alpha + gamma_I)*I(t)),
+    sympy.Eq(A(t).diff(t), sigma*(1 - rho)*E(t) - gamma_A*A(t)),
+    sympy.Eq(S_q(t).diff(t), (1 - beta)*c(t)*q*S(t)*(I(t) + theta*A(t)) - lambda_*S_q(t)),
+    sympy.Eq(E_q(t).diff(t), beta*c(t)*q*S(t)*(I(t) + theta*A(t)) - delta_q*E_q(t)),
+    sympy.Eq(H(t).diff(t), delta_I(t)*I(t) + delta_q*E_q(t) - (alpha + gamma_H)*H(t)),
+    sympy.Eq(R(t).diff(t), gamma_I*I(t) + gamma_A*A(t) + gamma_H*H(t))
+]</t>
+  </si>
+  <si>
+    <t>odes = [
+    sympy.Eq(S(t).diff(t), Lambda - mu*S(t) - beta*S(t)*I(t)/N),
+    sympy.Eq(E(t).diff(t), beta*S(t)*I(t)/N - (mu + epsilon)*E(t)),
+    sympy.Eq(I(t).diff(t), epsilon*E(t) - (gamma + mu + alpha)*I(t)),
+    sympy.Eq(R(t).diff(t), gamma*I(t) - mu*R(t))
+]</t>
+  </si>
+  <si>
+    <t>odes = [
+    sympy.Eq(S(t).diff(t), Lambda_s - (beta_s + rho_s*(1 - beta_s))*epsilon_s*S(t)*I(t)/N - delta*S(t) + m_s*S_q(t)),
+    sympy.Eq(S_q(t).diff(t), (1 - beta_s)*epsilon_s*rho_s*S(t)*I(t)/N - (m_s + delta)*S_q(t)),
+    sympy.Eq(A(t).diff(t), beta_s*(1 - rho_s)*epsilon_s*S(t)*I(t)/N - (gamma_a + xi_a + delta)*A(t)),
+    sympy.Eq(I(t).diff(t), gamma_a*A(t) - (gamma_i + xi_i + delta)*I(t)),
+    sympy.Eq(I_q(t).diff(t), beta_s*epsilon_s*rho_s*S(t)*I(t)/N + gamma_i*I(t) - (xi_q + delta)*I_q(t)),
+    sympy.Eq(R(t).diff(t), xi_a*A(t) + xi_i*I(t) + xi_q*I_q(t) - delta*R(t))
+]</t>
+  </si>
+  <si>
+    <t>odes = [
+    sympy.Eq(S(t).diff(t), -(1 - epsilon)*beta*S(t)*I(t)/N),
+    sympy.Eq(E(t).diff(t), (1 - epsilon)*beta*S(t)*I(t)/N - sigma*E(t)),
+    sympy.Eq(I(t).diff(t), sigma*E(t) - gamma*I(t)),
+    sympy.Eq(R(t).diff(t), gamma*I(t))
+]</t>
+  </si>
+  <si>
+    <t>odes = [
+    sympy.Eq(S_c(t).diff(t), m(t)*S_u(t) - (1 - m(t))*S_c(t)),
+    sympy.Eq(S_u(t).diff(t), (1 - m(t))*S_c(t) - m(t)*S_u(t) - beta*(n*I_r(t) + I_u(t))*S_u(t) + theta*(1 - lambda_)*Q(t)),
+    sympy.Eq(E(t).diff(t), (1 - sigma)*beta*(n*I_r(t) + I_u(t))*S_u(t) - mu*E(t)),
+    sympy.Eq(I_r(t).diff(t), mu*f*E(t) + theta*lambda_*Q(t) - eta_r*I_r(t)),
+    sympy.Eq(I_u(t).diff(t), mu*(1 - f)*E(t) - eta_u*I_u(t)),
+    sympy.Eq(R(t).diff(t), eta_r*q*I_r(t) + eta_u*I_u(t)),
+    sympy.Eq(Q(t).diff(t), sigma*beta*(n*I_r(t) + I_u(t))*S_u(t) - theta*Q(t))
+]</t>
+  </si>
+  <si>
+    <t>odes = [
+    sympy.Eq(S(t).diff(t), -beta*S(t)/N*I(t)),
+    sympy.Eq(E(t).diff(t), beta*S(t)/N*I(t) - omega*E(t)),
+    sympy.Eq(I(t).diff(t), omega*E(t) - gamma*I(t)),
+    sympy.Eq(R(t).diff(t), gamma*I(t))
+]</t>
+  </si>
+  <si>
+    <t>odes = [
+    sympy.Eq(S(t).diff(t), -beta_c*(alpha*A(t) + I(t))*S(t)/(N_h - I_D(t))),
+    sympy.Eq(E(t).diff(t), beta_c*(alpha*A(t) + I(t))*S(t)/(N_h - I_D(t)) - sigma*E(t)),
+    sympy.Eq(A(t).diff(t), nu*sigma*E(t) - (theta + gamma_a)*A(t)),
+    sympy.Eq(I(t).diff(t), (1 - nu)*sigma*E(t) - (psi + gamma_O + d_O)*I(t)),
+    sympy.Eq(I_D(t).diff(t), theta*A(t) + psi*I(t) - (gamma_i + d_D)*I_D(t)),
+    sympy.Eq(R(t).diff(t), gamma_i*I_D(t) + gamma_a*A(t) + gamma_O*I(t))
 ]</t>
   </si>
   <si>
     <t>odes = [
     sympy.Eq(S(t).diff(t), -beta(t)*S(t)/N*I(t) + omega*R(t)),
-    sympy.Eq(E(t).diff(t), beta(t)*S(t)*/N*I(t) - sigma*E(t)),
+    sympy.Eq(E(t).diff(t), beta(t)*S(t)/N*I(t) - sigma*E(t)),
     sympy.Eq(I(t).diff(t), sigma*E(t) - gamma*I(t)),
     sympy.Eq(R(t).diff(t), gamma*I(t) - omega*R(t))
 ]</t>
-  </si>
-  <si>
-    <t>BIOMD0000000984</t>
-  </si>
-  <si>
-    <t>odes = [
-    sympy.Eq(S_c(t).diff(t), m(t)*S_u - (1 - m(t))*S_c),
-    sympy.Eq(S_u(t).diff(t), (1 - m(t))*S_c - m(t)*S_u - beta*(n*I_r + I_u)*S_u + theta*(1 - lambda_)*Q),
-    sympy.Eq(E(t).diff(t), (1 - sigma)*beta*(n*I_r + I_u)*S_u - mu*E),
-    sympy.Eq(I_r(t).diff(t), mu*f*E + theta*lambda*Q - eta_r*I_r),
-    sympy.Eq(I_u(t).diff(t), mu*(1 - f)*E - eta_u*I_u),
-    sympy.Eq(R(t).diff(t), eta_r*q*I_r + eta_u*I_u),
-    sympy.Eq(Q(t).diff(t), sigma*beta*(n*I_r + I_u)*S_u - theta*Q)
-]</t>
-  </si>
-  <si>
-    <t>BIOMD0000000983</t>
-  </si>
-  <si>
-    <t>odes = [
-    sympy.Eq(S(t).diff(t), -beta*S/N*I),
-    sympy.Eq(E(t).diff(t), beta*S/N*I - omega*E),
-    sympy.Eq(I(t).diff(t), omega*E - gamma*I),
-    sympy.Eq(R(t).diff(t), gamma*I)
-]</t>
-  </si>
-  <si>
-    <t>odes = [
-    sympy.Eq(S(t).diff(t), -beta_c*(alpha*A + I)*S/(N_h - I_D)),
-    sympy.Eq(E(t).diff(t), beta_c*(alpha*A + I)*S/(N_h - I_D) - sigma*E),
-    sympy.Eq(A(t).diff(t), nu*sigma*E - (theta + gamma_a)*A),
-    sympy.Eq(I(t).diff(t), (1 - nu)*sigma*E - (psi + gamma_O + d_O)*I),
-    sympy.Eq(I_D(t).diff(t), theta*A + psi*I - (gamma_i + d_D)*I_D),
-    sympy.Eq(R(t).diff(t), gamma_i*I_D + gamma_a*A + gamma_O*I)
-]</t>
-  </si>
-  <si>
-    <t>BIOMD0000000991</t>
   </si>
 </sst>
 </file>
@@ -738,8 +738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{585F8C20-F92E-4147-81E7-1FDA03FC9F94}">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -843,92 +843,92 @@
         <v>22</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="221" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" ht="170" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+      <c r="B13" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="119" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B14" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="187" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" ht="102" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+      <c r="B15" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="204" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="170" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="187" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="B16" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="102" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="119" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="187" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="204" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="102" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="102" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="170" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="102" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>45</v>
@@ -936,7 +936,7 @@
     </row>
     <row r="24" spans="1:2" ht="136" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>46</v>

</xml_diff>